<commit_message>
Finish initial version of the code.
</commit_message>
<xml_diff>
--- a/SmartApps/temp_to_color.xlsx
+++ b/SmartApps/temp_to_color.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="42">
   <si>
     <t>Temp Colors</t>
   </si>
@@ -138,13 +138,25 @@
   </si>
   <si>
     <t>yellow</t>
+  </si>
+  <si>
+    <t>pink</t>
+  </si>
+  <si>
+    <t>App Weather</t>
+  </si>
+  <si>
+    <t>App color</t>
+  </si>
+  <si>
+    <t>App Hue Code</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -155,6 +167,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -180,11 +200,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,32 +486,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="22.7109375" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="8" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" customWidth="1"/>
     <col min="12" max="12" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E2" s="1" t="s">
         <v>11</v>
       </c>
@@ -503,8 +536,11 @@
       <c r="I2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -520,8 +556,14 @@
       <c r="H3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -540,8 +582,11 @@
       <c r="I4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -560,8 +605,11 @@
       <c r="I5" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -580,8 +628,11 @@
       <c r="I6" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -595,7 +646,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -609,7 +660,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -623,7 +674,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -637,7 +688,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -651,7 +702,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -665,7 +716,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E13" s="1" t="s">
         <v>22</v>
       </c>
@@ -673,7 +724,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E14" s="1" t="s">
         <v>23</v>
       </c>
@@ -681,7 +732,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E15" s="1" t="s">
         <v>24</v>
       </c>
@@ -689,7 +740,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E16" s="1" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
Fixed a couple bugs after resting.
</commit_message>
<xml_diff>
--- a/SmartApps/temp_to_color.xlsx
+++ b/SmartApps/temp_to_color.xlsx
@@ -134,9 +134,6 @@
     <t>orange</t>
   </si>
   <si>
-    <t>blue</t>
-  </si>
-  <si>
     <t>yellow</t>
   </si>
   <si>
@@ -150,6 +147,9 @@
   </si>
   <si>
     <t>App Hue Code</t>
+  </si>
+  <si>
+    <t>green</t>
   </si>
 </sst>
 </file>
@@ -489,7 +489,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,13 +514,13 @@
         <v>33</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -534,7 +534,7 @@
         <v>28</v>
       </c>
       <c r="I2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J2">
         <v>25</v>
@@ -557,10 +557,10 @@
         <v>17</v>
       </c>
       <c r="I3" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="J3">
-        <v>83</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -626,10 +626,10 @@
         <v>27</v>
       </c>
       <c r="I6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J6">
-        <v>70</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>